<commit_message>
added more csv files to visualization data
</commit_message>
<xml_diff>
--- a/data_for_visualizations/SelectedData.xlsx
+++ b/data_for_visualizations/SelectedData.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="implicitVSexplicit_by_year" sheetId="1" r:id="rId1"/>
     <sheet name="implicitVSexplicit_by_5_years" sheetId="2" r:id="rId2"/>
+    <sheet name="implicitVSexplicit_by_country" sheetId="5" r:id="rId3"/>
+    <sheet name="char_sexuality_general" sheetId="3" r:id="rId4"/>
+    <sheet name="char_sexuality_by_country" sheetId="4" r:id="rId5"/>
+    <sheet name="homophobia_transphobia" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>year</t>
   </si>
@@ -61,13 +65,106 @@
   </si>
   <si>
     <t>2011-Today</t>
+  </si>
+  <si>
+    <t>gay</t>
+  </si>
+  <si>
+    <t>lesbian</t>
+  </si>
+  <si>
+    <t>bisexual</t>
+  </si>
+  <si>
+    <t>asexual</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t>belgium</t>
+  </si>
+  <si>
+    <t>canada</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>germany</t>
+  </si>
+  <si>
+    <t>japan</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>norway</t>
+  </si>
+  <si>
+    <t>spain</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>italy</t>
+  </si>
+  <si>
+    <t>poland</t>
+  </si>
+  <si>
+    <t>south korea</t>
+  </si>
+  <si>
+    <t>singapore</t>
+  </si>
+  <si>
+    <t>homophobia</t>
+  </si>
+  <si>
+    <t>transphobia</t>
+  </si>
+  <si>
+    <t>NPC</t>
+  </si>
+  <si>
+    <t>playable</t>
+  </si>
+  <si>
+    <t>total_num_games</t>
+  </si>
+  <si>
+    <t>queer_man</t>
+  </si>
+  <si>
+    <t>queer_woman</t>
+  </si>
+  <si>
+    <t>rumoured</t>
+  </si>
+  <si>
+    <t>optional_relationships</t>
+  </si>
+  <si>
+    <t>prostitution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,6 +200,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -121,25 +230,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,21 +558,6 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -473,25 +577,8 @@
         <f>C2/(B2+C2)</f>
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <f>SUM(B2:B6)</f>
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <f>SUM(C2:C6)</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <f>H2/(I2+H2)</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="3">
-        <f>I2/(H2+I2)</f>
-        <v>0</v>
-      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -509,25 +596,8 @@
       <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3">
-        <f>SUM(B7:B11)</f>
-        <v>15</v>
-      </c>
-      <c r="I3">
-        <f>SUM(C7:C11)</f>
-        <v>5</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" ref="J3:J7" si="0">H3/(I3+H3)</f>
-        <v>0.75</v>
-      </c>
-      <c r="K3" s="3">
-        <f t="shared" ref="K3:K7" si="1">I3/(H3+I3)</f>
-        <v>0.25</v>
-      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -540,32 +610,15 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D3:D32" si="2">(B4)/(B4+C4)</f>
+        <f t="shared" ref="D3:D32" si="0">(B4)/(B4+C4)</f>
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E3:E32" si="3">C4/(B4+C4)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <f>SUM(B12:B16)</f>
-        <v>27</v>
-      </c>
-      <c r="I4">
-        <f>SUM(C12:C16)</f>
-        <v>18</v>
-      </c>
-      <c r="J4" s="3">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="K4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
+        <f t="shared" ref="E3:E32" si="1">C4/(B4+C4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -578,32 +631,15 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <f>SUM(B17:B21)</f>
-        <v>58</v>
-      </c>
-      <c r="I5">
-        <f>SUM(C17:C21)</f>
-        <v>49</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.54205607476635509</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.45794392523364486</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -616,32 +652,15 @@
         <v>0</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <f>SUM(B22:B26)</f>
-        <v>63</v>
-      </c>
-      <c r="I6">
-        <f>SUM(C22:C26)</f>
-        <v>34</v>
-      </c>
-      <c r="J6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.64948453608247425</v>
-      </c>
-      <c r="K6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.35051546391752575</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -654,32 +673,17 @@
         <v>0</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="2">
-        <f>SUM(B27:B32)</f>
-        <v>51</v>
-      </c>
-      <c r="I7" s="2">
-        <f>SUM(C27:C32)</f>
-        <v>6</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.89473684210526316</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.10526315789473684</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -692,11 +696,11 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -711,11 +715,11 @@
         <v>2</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -730,11 +734,11 @@
         <v>0</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -749,11 +753,11 @@
         <v>3</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -768,11 +772,11 @@
         <v>1</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -787,11 +791,11 @@
         <v>6</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -806,11 +810,11 @@
         <v>2</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -825,11 +829,11 @@
         <v>3</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
     </row>
@@ -844,11 +848,11 @@
         <v>6</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
     </row>
@@ -863,11 +867,11 @@
         <v>4</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.76470588235294112</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
     </row>
@@ -882,11 +886,11 @@
         <v>7</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -901,11 +905,11 @@
         <v>9</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
     </row>
@@ -920,11 +924,11 @@
         <v>16</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.4838709677419355</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.5161290322580645</v>
       </c>
     </row>
@@ -939,11 +943,11 @@
         <v>13</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
     </row>
@@ -958,11 +962,11 @@
         <v>2</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -977,11 +981,11 @@
         <v>7</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
     </row>
@@ -996,11 +1000,11 @@
         <v>15</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.54545454545454541</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.45454545454545453</v>
       </c>
     </row>
@@ -1015,11 +1019,11 @@
         <v>7</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.46666666666666667</v>
       </c>
     </row>
@@ -1034,11 +1038,11 @@
         <v>3</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.91428571428571426</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -1053,11 +1057,11 @@
         <v>1</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1072,11 +1076,11 @@
         <v>0</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1091,11 +1095,11 @@
         <v>0</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1110,11 +1114,11 @@
         <v>1</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1129,11 +1133,11 @@
         <v>1</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.875</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
     </row>
@@ -1148,11 +1152,11 @@
         <v>3</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1166,7 +1170,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E7" sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,4 +1297,1324 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1">
+        <v>89</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1985</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1986</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1987</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B14" s="1">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B18" s="1">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B21" s="1">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B22" s="1">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B25" s="1">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B26" s="1">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B27" s="1">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B29" s="1">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B31" s="1">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1">
+        <v>56</v>
+      </c>
+      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1">
+        <v>51</v>
+      </c>
+      <c r="D16" s="1">
+        <v>30</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.4">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5">
+        <v>41</v>
+      </c>
+      <c r="C2" s="6">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more data for visualizations
</commit_message>
<xml_diff>
--- a/data_for_visualizations/SelectedData.xlsx
+++ b/data_for_visualizations/SelectedData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="implicitVSexplicit_by_year" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="char_sexuality_general" sheetId="3" r:id="rId4"/>
     <sheet name="char_sexuality_by_country" sheetId="4" r:id="rId5"/>
     <sheet name="homophobia_transphobia" sheetId="6" r:id="rId6"/>
+    <sheet name="char_gender_by_country" sheetId="7" r:id="rId7"/>
+    <sheet name="char_sexuality_by_genre" sheetId="8" r:id="rId8"/>
+    <sheet name="genre_by_year" sheetId="9" r:id="rId9"/>
+    <sheet name="genre_by_decade" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="58">
   <si>
     <t>year</t>
   </si>
@@ -145,26 +149,74 @@
     <t>total_num_games</t>
   </si>
   <si>
-    <t>queer_man</t>
-  </si>
-  <si>
-    <t>queer_woman</t>
-  </si>
-  <si>
-    <t>rumoured</t>
-  </si>
-  <si>
-    <t>optional_relationships</t>
-  </si>
-  <si>
-    <t>prostitution</t>
+    <t>characters</t>
+  </si>
+  <si>
+    <t>relationships</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>actions and others</t>
+  </si>
+  <si>
+    <t>enemies</t>
+  </si>
+  <si>
+    <t>char role</t>
+  </si>
+  <si>
+    <t>queer and others</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>trans</t>
+  </si>
+  <si>
+    <t>non-binary</t>
+  </si>
+  <si>
+    <t>non-conforming</t>
+  </si>
+  <si>
+    <t>cis</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>adventure</t>
+  </si>
+  <si>
+    <t>fighting</t>
+  </si>
+  <si>
+    <t>rpg</t>
+  </si>
+  <si>
+    <t>shooter</t>
+  </si>
+  <si>
+    <t>simulation</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>decade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,6 +264,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,7 +287,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -240,8 +297,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -249,16 +314,32 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -610,11 +691,11 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D3:D32" si="0">(B4)/(B4+C4)</f>
+        <f t="shared" ref="D4:D32" si="0">(B4)/(B4+C4)</f>
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E3:E32" si="1">C4/(B4+C4)</f>
+        <f t="shared" ref="E4:E32" si="1">C4/(B4+C4)</f>
         <v>0</v>
       </c>
       <c r="J4" s="3"/>
@@ -1158,6 +1239,136 @@
       <c r="E32" s="4">
         <f t="shared" si="1"/>
         <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1980</v>
+      </c>
+      <c r="B2" s="2">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1990</v>
+      </c>
+      <c r="B3" s="2">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>98</v>
+      </c>
+      <c r="C4" s="2">
+        <v>176</v>
+      </c>
+      <c r="D4" s="2">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2">
+        <v>49</v>
+      </c>
+      <c r="G4" s="2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B5" s="2">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2">
+        <v>139</v>
+      </c>
+      <c r="D5" s="2">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1515,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1477,15 +1688,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A33"/>
+      <selection activeCell="A2" sqref="A2:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1504,8 +1715,11 @@
       <c r="F1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1985</v>
       </c>
@@ -1524,8 +1738,12 @@
       <c r="F2" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <f>SUM(B2:F2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1986</v>
       </c>
@@ -1544,8 +1762,12 @@
       <c r="F3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <f t="shared" ref="G3:G33" si="0">SUM(B3:F3)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1987</v>
       </c>
@@ -1564,8 +1786,12 @@
       <c r="F4" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1988</v>
       </c>
@@ -1584,8 +1810,12 @@
       <c r="F5" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1989</v>
       </c>
@@ -1604,8 +1834,12 @@
       <c r="F6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1990</v>
       </c>
@@ -1624,8 +1858,12 @@
       <c r="F7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1991</v>
       </c>
@@ -1644,8 +1882,12 @@
       <c r="F8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1992</v>
       </c>
@@ -1664,8 +1906,12 @@
       <c r="F9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1993</v>
       </c>
@@ -1684,8 +1930,12 @@
       <c r="F10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1994</v>
       </c>
@@ -1704,8 +1954,12 @@
       <c r="F11" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1995</v>
       </c>
@@ -1724,8 +1978,12 @@
       <c r="F12" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1996</v>
       </c>
@@ -1744,8 +2002,12 @@
       <c r="F13" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1997</v>
       </c>
@@ -1764,8 +2026,12 @@
       <c r="F14" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1998</v>
       </c>
@@ -1784,8 +2050,12 @@
       <c r="F15" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1999</v>
       </c>
@@ -1804,8 +2074,12 @@
       <c r="F16" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2000</v>
       </c>
@@ -1824,8 +2098,12 @@
       <c r="F17" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2001</v>
       </c>
@@ -1844,8 +2122,12 @@
       <c r="F18" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2002</v>
       </c>
@@ -1864,8 +2146,12 @@
       <c r="F19" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2003</v>
       </c>
@@ -1884,8 +2170,12 @@
       <c r="F20" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2004</v>
       </c>
@@ -1904,8 +2194,12 @@
       <c r="F21" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2005</v>
       </c>
@@ -1924,8 +2218,12 @@
       <c r="F22" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2006</v>
       </c>
@@ -1944,8 +2242,12 @@
       <c r="F23" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2007</v>
       </c>
@@ -1964,8 +2266,12 @@
       <c r="F24" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2008</v>
       </c>
@@ -1984,8 +2290,12 @@
       <c r="F25" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2009</v>
       </c>
@@ -2004,8 +2314,12 @@
       <c r="F26" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2010</v>
       </c>
@@ -2024,8 +2338,12 @@
       <c r="F27" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2011</v>
       </c>
@@ -2044,8 +2362,12 @@
       <c r="F28" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2012</v>
       </c>
@@ -2064,8 +2386,12 @@
       <c r="F29" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2013</v>
       </c>
@@ -2084,8 +2410,12 @@
       <c r="F30" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2014</v>
       </c>
@@ -2104,8 +2434,12 @@
       <c r="F31" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2015</v>
       </c>
@@ -2124,8 +2458,12 @@
       <c r="F32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2016</v>
       </c>
@@ -2143,6 +2481,10 @@
       </c>
       <c r="F33" s="1">
         <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2155,7 +2497,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection sqref="A1:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2164,7 +2506,7 @@
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2181,10 +2523,13 @@
         <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2203,8 +2548,12 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <f>SUM(B2:F2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -2223,8 +2572,12 @@
       <c r="F3" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <f t="shared" ref="G3:G16" si="0">SUM(B3:F3)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -2243,8 +2596,12 @@
       <c r="F4" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -2263,8 +2620,12 @@
       <c r="F5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2283,8 +2644,12 @@
       <c r="F6" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2303,8 +2668,12 @@
       <c r="F7" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -2323,8 +2692,12 @@
       <c r="F8" s="1">
         <v>160</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -2343,8 +2716,12 @@
       <c r="F9" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -2363,8 +2740,12 @@
       <c r="F10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -2383,8 +2764,12 @@
       <c r="F11" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -2403,8 +2788,12 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -2423,8 +2812,12 @@
       <c r="F13" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -2443,8 +2836,12 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -2463,8 +2860,12 @@
       <c r="F15" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -2482,6 +2883,10 @@
       </c>
       <c r="F16" s="1">
         <v>184</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -2558,61 +2963,2086 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" customWidth="1"/>
+    <col min="13" max="13" width="27.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="G1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="34" x14ac:dyDescent="0.4">
+      <c r="A3" s="7">
+        <v>861</v>
+      </c>
+      <c r="B3" s="5">
+        <v>93</v>
+      </c>
+      <c r="C3" s="5">
+        <f>A3-(B3+D3)</f>
+        <v>243</v>
+      </c>
+      <c r="D3" s="5">
+        <v>525</v>
+      </c>
+      <c r="E3" s="5">
+        <v>41</v>
+      </c>
+      <c r="F3" s="6">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5">
+        <v>738</v>
+      </c>
+      <c r="H3" s="5">
+        <v>96</v>
+      </c>
+      <c r="I3" s="5">
+        <v>27</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="5:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="5:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="5:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1">
+        <v>52</v>
+      </c>
+      <c r="C2">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>104</v>
+      </c>
+      <c r="G2" s="1">
+        <f>SUM(B2:E2)</f>
+        <v>101</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>42</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>206</v>
+      </c>
+      <c r="G3" s="1">
+        <f>SUM(B3:E3)</f>
+        <v>144</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1">
+        <f>SUM(B4:E4)</f>
+        <v>16</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1">
+        <f>SUM(B5:E5)</f>
+        <v>10</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+      <c r="G6" s="1">
+        <f>SUM(B6:E6)</f>
+        <v>17</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>103</v>
+      </c>
+      <c r="G7" s="1">
+        <f>SUM(B7:E7)</f>
+        <v>81</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1">
+        <f>SUM(B2:B7)</f>
+        <v>179</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(C2:C7)</f>
+        <v>85</v>
+      </c>
+      <c r="D9" s="1">
+        <f>SUM(D2:D7)</f>
+        <v>103</v>
+      </c>
+      <c r="E9" s="1">
+        <f>SUM(E2:E7)</f>
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SUM(F2:F7)</f>
+        <v>525</v>
+      </c>
+      <c r="G9" s="1">
+        <f>SUM(G2:G7)</f>
+        <v>369</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="9">
+        <f>B2/B$9</f>
+        <v>0.29050279329608941</v>
+      </c>
+      <c r="C11" s="10">
+        <f>C2/C$9</f>
+        <v>0.27058823529411763</v>
+      </c>
+      <c r="D11" s="10">
+        <f>D2/D$9</f>
+        <v>0.25242718446601942</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="9">
+        <f>B2/G2</f>
+        <v>0.51485148514851486</v>
+      </c>
+      <c r="I11" s="10">
+        <f>C2/G2</f>
+        <v>0.22772277227722773</v>
+      </c>
+      <c r="J11" s="10">
+        <f>D2/G2</f>
+        <v>0.25742574257425743</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="9">
+        <f>B3/B$9</f>
+        <v>0.35195530726256985</v>
+      </c>
+      <c r="C12" s="10">
+        <f>C3/C$9</f>
+        <v>0.44705882352941179</v>
+      </c>
+      <c r="D12" s="10">
+        <f>D3/D$9</f>
+        <v>0.40776699029126212</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="9">
+        <f>B3/G3</f>
+        <v>0.4375</v>
+      </c>
+      <c r="I12" s="10">
+        <f>C3/G3</f>
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="J12" s="10">
+        <f>D3/G3</f>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="9">
+        <f>B4/B$9</f>
+        <v>3.3519553072625698E-2</v>
+      </c>
+      <c r="C13" s="10">
+        <f>C4/C$9</f>
+        <v>7.0588235294117646E-2</v>
+      </c>
+      <c r="D13" s="10">
+        <f>D4/D$9</f>
+        <v>3.8834951456310676E-2</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="9">
+        <f>B4/G4</f>
+        <v>0.375</v>
+      </c>
+      <c r="I13" s="10">
+        <f>C4/G4</f>
+        <v>0.375</v>
+      </c>
+      <c r="J13" s="10">
+        <f>D4/G4</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="9">
+        <f>B5/B$9</f>
+        <v>3.9106145251396648E-2</v>
+      </c>
+      <c r="C14" s="10">
+        <f>C5/C$9</f>
+        <v>1.1764705882352941E-2</v>
+      </c>
+      <c r="D14" s="10">
+        <f>D5/D$9</f>
+        <v>1.9417475728155338E-2</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="9">
+        <f>B5/G5</f>
+        <v>0.7</v>
+      </c>
+      <c r="I14" s="10">
+        <f>C5/G5</f>
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="10">
+        <f>D5/G5</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="9">
+        <f>B6/B$9</f>
+        <v>6.1452513966480445E-2</v>
+      </c>
+      <c r="C15" s="10">
+        <f>C6/C$9</f>
+        <v>4.7058823529411764E-2</v>
+      </c>
+      <c r="D15" s="10">
+        <f>D6/D$9</f>
+        <v>9.7087378640776691E-3</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="9">
+        <f>B6/G6</f>
+        <v>0.6470588235294118</v>
+      </c>
+      <c r="I15" s="10">
+        <f>C6/G6</f>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="J15" s="10">
+        <f>D6/G6</f>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="9">
+        <f>B7/B$9</f>
+        <v>0.22346368715083798</v>
+      </c>
+      <c r="C16" s="10">
+        <f>C7/C$9</f>
+        <v>0.15294117647058825</v>
+      </c>
+      <c r="D16" s="10">
+        <f>D7/D$9</f>
+        <v>0.27184466019417475</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="9">
+        <f>B7/G7</f>
+        <v>0.49382716049382713</v>
+      </c>
+      <c r="I16" s="10">
+        <f>C7/G7</f>
+        <v>0.16049382716049382</v>
+      </c>
+      <c r="J16" s="10">
+        <f>D7/G7</f>
+        <v>0.34567901234567899</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="1">
+        <v>51</v>
+      </c>
+      <c r="I18">
+        <v>23</v>
+      </c>
+      <c r="J18">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>41</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="1">
+        <v>44</v>
+      </c>
+      <c r="I19">
+        <v>26</v>
+      </c>
+      <c r="J19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="1">
+        <v>38</v>
+      </c>
+      <c r="I20">
+        <v>38</v>
+      </c>
+      <c r="J20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="1">
+        <v>70</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="1">
+        <v>65</v>
+      </c>
+      <c r="I22">
+        <v>24</v>
+      </c>
+      <c r="J22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="1">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>27</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="1">
+        <v>49</v>
+      </c>
+      <c r="I23">
+        <v>16</v>
+      </c>
+      <c r="J23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="11">
+        <f>B18/B$19  *5</f>
+        <v>4.1428571428571432</v>
+      </c>
+      <c r="C25" s="12">
+        <f>C18/C$19 * 5</f>
+        <v>3</v>
+      </c>
+      <c r="D25" s="12">
+        <f>D18/D$19 * 5</f>
+        <v>3.0487804878048781</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="12">
+        <f>H18/H$22 * 5</f>
+        <v>3.9230769230769229</v>
+      </c>
+      <c r="I25" s="12">
+        <f>I18/I$20 * 5</f>
+        <v>3.0263157894736841</v>
+      </c>
+      <c r="J25" s="12">
+        <f>J18/J$23 * 5</f>
+        <v>3.7142857142857144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="11">
+        <f>B19/B$19  *5</f>
+        <v>5</v>
+      </c>
+      <c r="C26" s="12">
+        <f>C19/C$19 * 5</f>
+        <v>5</v>
+      </c>
+      <c r="D26" s="12">
+        <f>D19/D$19 * 5</f>
+        <v>5</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="12">
+        <f>H19/H$22 * 5</f>
+        <v>3.384615384615385</v>
+      </c>
+      <c r="I26" s="12">
+        <f>I19/I$20 * 5</f>
+        <v>3.4210526315789473</v>
+      </c>
+      <c r="J26" s="12">
+        <f>J19/J$23 * 5</f>
+        <v>4.1428571428571432</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="11">
+        <f>B20/B$19  *5</f>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="C27" s="12">
+        <f>C20/C$19 * 5</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D27" s="12">
+        <f>D20/D$19 * 5</f>
+        <v>0.48780487804878048</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="12">
+        <f>H20/H$22 * 5</f>
+        <v>2.9230769230769234</v>
+      </c>
+      <c r="I27" s="12">
+        <f>I20/I$20 * 5</f>
+        <v>5</v>
+      </c>
+      <c r="J27" s="12">
+        <f>J20/J$23 * 5</f>
+        <v>3.5714285714285716</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="11">
+        <f>B21/B$19  *5</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="C28" s="12">
+        <f>C21/C$19 * 5</f>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="D28" s="12">
+        <f>D21/D$19 * 5</f>
+        <v>0.24390243902439024</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="12">
+        <f>H21/H$22 * 5</f>
+        <v>5.3846153846153841</v>
+      </c>
+      <c r="I28" s="12">
+        <f>I21/I$20 * 5</f>
+        <v>1.3157894736842104</v>
+      </c>
+      <c r="J28" s="12">
+        <f>J21/J$23 * 5</f>
+        <v>2.8571428571428568</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="11">
+        <f>B22/B$19  *5</f>
+        <v>0.85714285714285721</v>
+      </c>
+      <c r="C29" s="12">
+        <f>C22/C$19 * 5</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D29" s="12">
+        <f>D22/D$19 * 5</f>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="12">
+        <f>H22/H$22 * 5</f>
+        <v>5</v>
+      </c>
+      <c r="I29" s="12">
+        <f>I22/I$20 * 5</f>
+        <v>3.1578947368421053</v>
+      </c>
+      <c r="J29" s="12">
+        <f>J22/J$23 * 5</f>
+        <v>0.85714285714285721</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="11">
+        <f>B23/B$19  *5</f>
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="C30" s="12">
+        <f>C23/C$19 * 5</f>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="D30" s="12">
+        <f>D23/D$19 * 5</f>
+        <v>3.2926829268292686</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="12">
+        <f>H23/H$22 * 5</f>
+        <v>3.7692307692307692</v>
+      </c>
+      <c r="I30" s="12">
+        <f>I23/I$20 * 5</f>
+        <v>2.1052631578947367</v>
+      </c>
+      <c r="J30" s="12">
+        <f>J23/J$23 * 5</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1985</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>80</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:Q2" si="0">SUM(B2:B6)</f>
+        <v>9</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1986</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>90</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:Q3" si="1">SUM(B7:B16)</f>
+        <v>52</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="N3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1987</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>2000</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:Q4" si="2">SUM(B17:B26)</f>
+        <v>98</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:Q5" si="3">SUM(B27:B33)</f>
+        <v>46</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>139</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B15" s="1">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
         <v>34</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.4">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5">
-        <v>41</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B21" s="1">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>4</v>
+      </c>
+      <c r="G22" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B23" s="1">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B25" s="1">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1">
         <v>33</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>4</v>
+      </c>
+      <c r="F25" s="1">
+        <v>9</v>
+      </c>
+      <c r="G25" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B26" s="1">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>15</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B27" s="1">
+        <v>16</v>
+      </c>
+      <c r="C27" s="1">
+        <v>34</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5</v>
+      </c>
+      <c r="G28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B30" s="1">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>5</v>
+      </c>
+      <c r="G30" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>9</v>
+      </c>
+      <c r="G31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added fullpage js library
</commit_message>
<xml_diff>
--- a/data_for_visualizations/SelectedData.xlsx
+++ b/data_for_visualizations/SelectedData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="implicitVSexplicit_by_year" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="70">
   <si>
     <t>year</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>traits</t>
+  </si>
+  <si>
+    <t>//DENDOGRAMA NOVO</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -318,8 +324,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -354,7 +364,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -363,6 +373,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -371,6 +383,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2624,7 +2638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2767,7 +2781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A33"/>
     </sheetView>
   </sheetViews>
@@ -4437,10 +4451,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5218,6 +5232,339 @@
         <v>5</v>
       </c>
     </row>
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="1">
+        <v>52</v>
+      </c>
+      <c r="C34" s="2">
+        <v>23</v>
+      </c>
+      <c r="D34" s="2">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <f>SUM(B34:D34)</f>
+        <v>101</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+    </row>
+    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="1">
+        <v>63</v>
+      </c>
+      <c r="C35" s="2">
+        <v>38</v>
+      </c>
+      <c r="D35" s="2">
+        <v>42</v>
+      </c>
+      <c r="E35">
+        <f>SUM(B35:D35)</f>
+        <v>143</v>
+      </c>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="1">
+        <v>6</v>
+      </c>
+      <c r="C36" s="2">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <f>SUM(B36:D36)</f>
+        <v>16</v>
+      </c>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="1">
+        <v>7</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <f>SUM(B37:D37)</f>
+        <v>10</v>
+      </c>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="1">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <f>SUM(B38:D38)</f>
+        <v>16</v>
+      </c>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="1">
+        <v>40</v>
+      </c>
+      <c r="C39" s="2">
+        <v>13</v>
+      </c>
+      <c r="D39" s="2">
+        <v>28</v>
+      </c>
+      <c r="E39">
+        <f>SUM(B39:D39)</f>
+        <v>81</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="1">
+        <v>52</v>
+      </c>
+      <c r="C43" s="1">
+        <v>63</v>
+      </c>
+      <c r="D43" s="1">
+        <v>6</v>
+      </c>
+      <c r="E43" s="1">
+        <v>7</v>
+      </c>
+      <c r="F43" s="1">
+        <v>11</v>
+      </c>
+      <c r="G43" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="2">
+        <v>23</v>
+      </c>
+      <c r="C44" s="2">
+        <v>38</v>
+      </c>
+      <c r="D44" s="2">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2">
+        <v>4</v>
+      </c>
+      <c r="G44" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="2">
+        <v>26</v>
+      </c>
+      <c r="C45" s="2">
+        <v>42</v>
+      </c>
+      <c r="D45" s="2">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2">
+        <v>2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="11">
+        <f>B43/B$43* 5</f>
+        <v>5</v>
+      </c>
+      <c r="C46" s="11">
+        <f>C43/C$43* 5</f>
+        <v>5</v>
+      </c>
+      <c r="D46" s="11">
+        <f>D43/D$43* 5</f>
+        <v>5</v>
+      </c>
+      <c r="E46" s="11">
+        <f>E43/E$43* 5</f>
+        <v>5</v>
+      </c>
+      <c r="F46" s="11">
+        <f>F43/F$43* 5</f>
+        <v>5</v>
+      </c>
+      <c r="G46" s="11">
+        <f>G43/G$43* 5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="11">
+        <f>B44/B$43* 5</f>
+        <v>2.2115384615384617</v>
+      </c>
+      <c r="C47" s="11">
+        <f>C44/C$43* 5</f>
+        <v>3.0158730158730158</v>
+      </c>
+      <c r="D47" s="11">
+        <f>D44/D$43* 5</f>
+        <v>5</v>
+      </c>
+      <c r="E47" s="11">
+        <f>E44/E$43* 5</f>
+        <v>0.71428571428571419</v>
+      </c>
+      <c r="F47" s="11">
+        <f>F44/F$43* 5</f>
+        <v>1.8181818181818183</v>
+      </c>
+      <c r="G47" s="11">
+        <f>G44/G$43* 5</f>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="11">
+        <f>B45/B$43* 5</f>
+        <v>2.5</v>
+      </c>
+      <c r="C48" s="11">
+        <f>C45/C$43* 5</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="D48" s="11">
+        <f>D45/D$43* 5</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="E48" s="11">
+        <f>E45/E$43* 5</f>
+        <v>1.4285714285714284</v>
+      </c>
+      <c r="F48" s="11">
+        <f>F45/F$43* 5</f>
+        <v>0.45454545454545459</v>
+      </c>
+      <c r="G48" s="11">
+        <f>G45/G$43* 5</f>
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>